<commit_message>
update manifest, fix datatable index
</commit_message>
<xml_diff>
--- a/Product Inventory.xlsx
+++ b/Product Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12140" yWindow="5840" windowWidth="28800" windowHeight="20440"/>
+    <workbookView xWindow="980" yWindow="2560" windowWidth="28800" windowHeight="20440"/>
   </bookViews>
   <sheets>
     <sheet name="Product Inventory" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A45"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>